<commit_message>
New reporting unit view (click on 2D map)
</commit_message>
<xml_diff>
--- a/app/04-kreise.xlsx
+++ b/app/04-kreise.xlsx
@@ -19625,8 +19625,8 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101004456E7D0170A5843A32AE86FB4FC254D" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f537ef4707253babc9c7e529a7fe617d">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9b0062f6-3850-45c4-a49c-48289d7656f5" xmlns:ns3="d4476a09-aef8-48ac-8c6f-fc751ea8799c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4de5c604fe36cfd17853a55eecc7430d" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101004456E7D0170A5843A32AE86FB4FC254D" ma:contentTypeVersion="15" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="235279f01f294a63ec87ee3004477524">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9b0062f6-3850-45c4-a49c-48289d7656f5" xmlns:ns3="d4476a09-aef8-48ac-8c6f-fc751ea8799c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1dda21a9530c309e182265077ef4719b" ns2:_="" ns3:_="">
     <xsd:import namespace="9b0062f6-3850-45c4-a49c-48289d7656f5"/>
     <xsd:import namespace="d4476a09-aef8-48ac-8c6f-fc751ea8799c"/>
     <xsd:element name="properties">
@@ -19647,6 +19647,8 @@
                 <xsd:element ref="ns2:MediaServiceAutoKeyPoints" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceKeyPoints" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
+                <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
+                <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -19711,11 +19713,18 @@
         <xsd:restriction base="dms:Unknown"/>
       </xsd:simpleType>
     </xsd:element>
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="21" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Bildmarkierungen" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="32a6b19d-68da-4000-ad0e-8ca94f8fa4c6" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
   </xsd:schema>
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="d4476a09-aef8-48ac-8c6f-fc751ea8799c" elementFormDefault="qualified">
     <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="SharedWithUsers" ma:index="10" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
+    <xsd:element name="SharedWithUsers" ma:index="10" nillable="true" ma:displayName="Freigegeben für" ma:internalName="SharedWithUsers" ma:readOnly="true">
       <xsd:complexType>
         <xsd:complexContent>
           <xsd:extension base="dms:UserMulti">
@@ -19734,12 +19743,23 @@
         </xsd:complexContent>
       </xsd:complexType>
     </xsd:element>
-    <xsd:element name="SharedWithDetails" ma:index="11" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
+    <xsd:element name="SharedWithDetails" ma:index="11" nillable="true" ma:displayName="Freigegeben für - Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note">
           <xsd:maxLength value="255"/>
         </xsd:restriction>
       </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="TaxCatchAll" ma:index="22" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{98ac2856-a420-4c13-9ab7-04832fcb732f}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="d4476a09-aef8-48ac-8c6f-fc751ea8799c">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
     </xsd:element>
   </xsd:schema>
   <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
@@ -19751,8 +19771,8 @@
         <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
-        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Inhaltstyp"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Titel"/>
         <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
         <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
@@ -19852,12 +19872,17 @@
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9b0062f6-3850-45c4-a49c-48289d7656f5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="d4476a09-aef8-48ac-8c6f-fc751ea8799c" xsi:nil="true"/>
+  </documentManagement>
 </p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D29EE0F2-4645-45AB-B1F3-FF69EE81D2FB}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3388B0AF-4144-44E0-BB33-C4E4884C3354}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>